<commit_message>
Menambahkan Slide Software , Kelebihan VR
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\TKPPL\Virtual-Reality-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -565,7 +565,7 @@
   <dimension ref="B4:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,9 @@
       <c r="I7" s="2">
         <v>0</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -689,7 +691,9 @@
       <c r="I8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -720,7 +724,9 @@
       <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -751,7 +757,9 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -782,7 +790,9 @@
       <c r="I11" s="2">
         <v>2</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -813,7 +823,9 @@
       <c r="I12" s="2">
         <v>3</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -844,7 +856,9 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -875,7 +889,9 @@
       <c r="I14" s="2">
         <v>5</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -906,7 +922,9 @@
       <c r="I15" s="2">
         <v>8</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2">
+        <v>8</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -937,7 +955,9 @@
       <c r="I16" s="2">
         <v>8</v>
       </c>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2">
+        <v>8</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -985,7 +1005,10 @@
         <f>H18-$F$18/10</f>
         <v>37.800000000000004</v>
       </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2">
+        <f>I18-$F$18/10</f>
+        <v>32.400000000000006</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1016,7 +1039,10 @@
         <f>SUM(I7:I16)</f>
         <v>36</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2">
+        <f>SUM(J7:J16)</f>
+        <v>25</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>

</xml_diff>